<commit_message>
manual uploading 2021/06/28 14:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/KAL.xlsx
+++ b/src/algorithms/plan_fact_module/KAL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="9">
   <si>
     <t>CarAmount</t>
   </si>
@@ -52,7 +52,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +80,20 @@
     <font>
       <sz val="9"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -113,11 +131,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -126,10 +149,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
+    <cellStyle name="Normal 3" xfId="5"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
+    <cellStyle name="Обычный 3" xfId="2"/>
+    <cellStyle name="Финансовый 2" xfId="3"/>
+    <cellStyle name="Финансовый 3" xfId="4"/>
+    <cellStyle name="Финансовый 4" xfId="6"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -407,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,11 +483,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>44317</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="A2" s="4">
+        <v>44287</v>
+      </c>
+      <c r="B2" s="6">
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -457,10 +500,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>44318</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="4">
+        <v>44288</v>
+      </c>
+      <c r="B3" s="6">
         <v>30</v>
       </c>
       <c r="C3" t="s">
@@ -474,10 +517,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="4">
+        <v>44289</v>
+      </c>
+      <c r="B4" s="6">
         <v>30</v>
       </c>
       <c r="C4" t="s">
@@ -491,11 +534,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
+      <c r="A5" s="4">
+        <v>44290</v>
+      </c>
+      <c r="B5" s="6">
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -508,10 +551,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>44321</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="4">
+        <v>44291</v>
+      </c>
+      <c r="B6" s="6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
@@ -525,284 +568,284 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>44322</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="4">
+        <v>44292</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>44293</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>44294</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>44295</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>44296</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>44297</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>44298</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>44299</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>44300</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>44301</v>
+      </c>
+      <c r="B16" s="6">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>44323</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>44302</v>
+      </c>
+      <c r="B17" s="6">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>44324</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>44303</v>
+      </c>
+      <c r="B18" s="6">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>44325</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>44304</v>
+      </c>
+      <c r="B19" s="6">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>44326</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>44327</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>44305</v>
+      </c>
+      <c r="B20" s="6">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>44328</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>44306</v>
+      </c>
+      <c r="B21" s="6">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>44329</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>44307</v>
+      </c>
+      <c r="B22" s="6">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>44330</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>44331</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>44308</v>
+      </c>
+      <c r="B23" s="6">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>44332</v>
-      </c>
-      <c r="B17" s="2">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>44333</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>44334</v>
-      </c>
-      <c r="B19" s="2">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>44335</v>
-      </c>
-      <c r="B20" s="2">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>44336</v>
-      </c>
-      <c r="B21" s="2">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>44337</v>
-      </c>
-      <c r="B22" s="2">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>44338</v>
-      </c>
-      <c r="B23" s="2">
-        <v>30</v>
-      </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
@@ -814,11 +857,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>44339</v>
-      </c>
-      <c r="B24" s="2">
-        <v>30</v>
+      <c r="A24" s="4">
+        <v>44309</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -831,10 +874,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>44340</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25" s="4">
+        <v>44310</v>
+      </c>
+      <c r="B25" s="6">
         <v>0</v>
       </c>
       <c r="C25" t="s">
@@ -848,11 +891,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>44341</v>
-      </c>
-      <c r="B26" s="2">
-        <v>30</v>
+      <c r="A26" s="4">
+        <v>44311</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -865,11 +908,11 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>44342</v>
-      </c>
-      <c r="B27" s="2">
-        <v>30</v>
+      <c r="A27" s="4">
+        <v>44312</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -882,10 +925,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>44343</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="A28" s="4">
+        <v>44313</v>
+      </c>
+      <c r="B28" s="6">
         <v>0</v>
       </c>
       <c r="C28" t="s">
@@ -899,11 +942,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>44344</v>
-      </c>
-      <c r="B29" s="2">
-        <v>30</v>
+      <c r="A29" s="4">
+        <v>44314</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -916,11 +959,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>44345</v>
-      </c>
-      <c r="B30" s="2">
-        <v>30</v>
+      <c r="A30" s="4">
+        <v>44315</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -933,11 +976,11 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>44346</v>
-      </c>
-      <c r="B31" s="2">
-        <v>30</v>
+      <c r="A31" s="4">
+        <v>44316</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -950,27 +993,27 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>44347</v>
-      </c>
-      <c r="B32" s="2">
-        <v>30</v>
+      <c r="A32" s="5">
+        <v>44287</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>44317</v>
-      </c>
-      <c r="B33" s="2">
+      <c r="A33" s="5">
+        <v>44288</v>
+      </c>
+      <c r="B33" s="7">
         <v>0</v>
       </c>
       <c r="C33" t="s">
@@ -984,10 +1027,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>44318</v>
-      </c>
-      <c r="B34" s="2">
+      <c r="A34" s="5">
+        <v>44289</v>
+      </c>
+      <c r="B34" s="7">
         <v>0</v>
       </c>
       <c r="C34" t="s">
@@ -1001,10 +1044,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B35" s="2">
+      <c r="A35" s="5">
+        <v>44290</v>
+      </c>
+      <c r="B35" s="7">
         <v>0</v>
       </c>
       <c r="C35" t="s">
@@ -1018,11 +1061,11 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0</v>
+      <c r="A36" s="5">
+        <v>44291</v>
+      </c>
+      <c r="B36" s="7">
+        <v>21</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -1035,11 +1078,11 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>44321</v>
-      </c>
-      <c r="B37" s="2">
-        <v>14</v>
+      <c r="A37" s="5">
+        <v>44292</v>
+      </c>
+      <c r="B37" s="7">
+        <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
@@ -1052,11 +1095,11 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>44322</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0</v>
+      <c r="A38" s="5">
+        <v>44293</v>
+      </c>
+      <c r="B38" s="7">
+        <v>21</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -1069,11 +1112,11 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>44323</v>
-      </c>
-      <c r="B39" s="2">
-        <v>0</v>
+      <c r="A39" s="5">
+        <v>44294</v>
+      </c>
+      <c r="B39" s="7">
+        <v>21</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -1086,11 +1129,11 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>44324</v>
-      </c>
-      <c r="B40" s="2">
-        <v>0</v>
+      <c r="A40" s="5">
+        <v>44295</v>
+      </c>
+      <c r="B40" s="7">
+        <v>21</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -1103,11 +1146,11 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>44325</v>
-      </c>
-      <c r="B41" s="2">
-        <v>0</v>
+      <c r="A41" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B41" s="7">
+        <v>21</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
@@ -1120,11 +1163,11 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>44326</v>
-      </c>
-      <c r="B42" s="2">
-        <v>0</v>
+      <c r="A42" s="5">
+        <v>44297</v>
+      </c>
+      <c r="B42" s="7">
+        <v>21</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -1137,11 +1180,11 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>44327</v>
-      </c>
-      <c r="B43" s="2">
-        <v>0</v>
+      <c r="A43" s="5">
+        <v>44298</v>
+      </c>
+      <c r="B43" s="7">
+        <v>21</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -1154,11 +1197,11 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>44328</v>
-      </c>
-      <c r="B44" s="2">
-        <v>0</v>
+      <c r="A44" s="5">
+        <v>44299</v>
+      </c>
+      <c r="B44" s="7">
+        <v>21</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -1171,11 +1214,11 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>44329</v>
-      </c>
-      <c r="B45" s="2">
-        <v>0</v>
+      <c r="A45" s="5">
+        <v>44300</v>
+      </c>
+      <c r="B45" s="8">
+        <v>35</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -1188,11 +1231,11 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>44330</v>
-      </c>
-      <c r="B46" s="2">
-        <v>14</v>
+      <c r="A46" s="5">
+        <v>44301</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
@@ -1205,10 +1248,10 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>44331</v>
-      </c>
-      <c r="B47" s="2">
+      <c r="A47" s="5">
+        <v>44302</v>
+      </c>
+      <c r="B47" s="7">
         <v>0</v>
       </c>
       <c r="C47" t="s">
@@ -1222,10 +1265,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>44332</v>
-      </c>
-      <c r="B48" s="2">
+      <c r="A48" s="5">
+        <v>44303</v>
+      </c>
+      <c r="B48" s="7">
         <v>0</v>
       </c>
       <c r="C48" t="s">
@@ -1239,11 +1282,11 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>44333</v>
-      </c>
-      <c r="B49" s="2">
-        <v>14</v>
+      <c r="A49" s="5">
+        <v>44304</v>
+      </c>
+      <c r="B49" s="7">
+        <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -1256,10 +1299,10 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>44334</v>
-      </c>
-      <c r="B50" s="2">
+      <c r="A50" s="5">
+        <v>44305</v>
+      </c>
+      <c r="B50" s="7">
         <v>0</v>
       </c>
       <c r="C50" t="s">
@@ -1273,10 +1316,10 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>44335</v>
-      </c>
-      <c r="B51" s="2">
+      <c r="A51" s="5">
+        <v>44306</v>
+      </c>
+      <c r="B51" s="7">
         <v>0</v>
       </c>
       <c r="C51" t="s">
@@ -1290,10 +1333,10 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>44336</v>
-      </c>
-      <c r="B52" s="2">
+      <c r="A52" s="5">
+        <v>44307</v>
+      </c>
+      <c r="B52" s="7">
         <v>0</v>
       </c>
       <c r="C52" t="s">
@@ -1307,10 +1350,10 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>44337</v>
-      </c>
-      <c r="B53" s="2">
+      <c r="A53" s="5">
+        <v>44308</v>
+      </c>
+      <c r="B53" s="7">
         <v>0</v>
       </c>
       <c r="C53" t="s">
@@ -1324,11 +1367,11 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>44338</v>
-      </c>
-      <c r="B54" s="2">
-        <v>0</v>
+      <c r="A54" s="5">
+        <v>44309</v>
+      </c>
+      <c r="B54" s="7">
+        <v>21</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -1341,11 +1384,11 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>44339</v>
-      </c>
-      <c r="B55" s="2">
-        <v>0</v>
+      <c r="A55" s="5">
+        <v>44310</v>
+      </c>
+      <c r="B55" s="7">
+        <v>21</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -1358,11 +1401,11 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>44340</v>
-      </c>
-      <c r="B56" s="2">
-        <v>14</v>
+      <c r="A56" s="5">
+        <v>44311</v>
+      </c>
+      <c r="B56" s="7">
+        <v>0</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
@@ -1375,10 +1418,10 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>44341</v>
-      </c>
-      <c r="B57" s="2">
+      <c r="A57" s="5">
+        <v>44312</v>
+      </c>
+      <c r="B57" s="7">
         <v>0</v>
       </c>
       <c r="C57" t="s">
@@ -1392,11 +1435,11 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>44342</v>
-      </c>
-      <c r="B58" s="2">
-        <v>0</v>
+      <c r="A58" s="5">
+        <v>44313</v>
+      </c>
+      <c r="B58" s="7">
+        <v>21</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
@@ -1409,11 +1452,11 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>44343</v>
-      </c>
-      <c r="B59" s="2">
-        <v>14</v>
+      <c r="A59" s="5">
+        <v>44314</v>
+      </c>
+      <c r="B59" s="7">
+        <v>21</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
@@ -1426,10 +1469,10 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>44344</v>
-      </c>
-      <c r="B60" s="2">
+      <c r="A60" s="5">
+        <v>44315</v>
+      </c>
+      <c r="B60" s="7">
         <v>0</v>
       </c>
       <c r="C60" t="s">
@@ -1443,10 +1486,10 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>44345</v>
-      </c>
-      <c r="B61" s="2">
+      <c r="A61" s="5">
+        <v>44316</v>
+      </c>
+      <c r="B61" s="7">
         <v>0</v>
       </c>
       <c r="C61" t="s">
@@ -1460,38 +1503,9 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>44346</v>
-      </c>
-      <c r="B62" s="2">
-        <v>0</v>
-      </c>
-      <c r="C62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>44347</v>
-      </c>
-      <c r="B63" s="2">
-        <v>0</v>
-      </c>
-      <c r="C63" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
+      <c r="E62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
manual uploading 2021/07/1 17:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/KAL.xlsx
+++ b/src/algorithms/plan_fact_module/KAL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="9">
   <si>
     <t>CarAmount</t>
   </si>
@@ -39,13 +39,13 @@
     <t>CargoEtsngName</t>
   </si>
   <si>
-    <t>КОНЦЕНТР МЕД</t>
-  </si>
-  <si>
     <t>Балхаш I</t>
   </si>
   <si>
     <t>Актогай</t>
+  </si>
+  <si>
+    <t>МЕДЬ</t>
   </si>
 </sst>
 </file>
@@ -140,16 +140,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:B63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,1057 +469,3339 @@
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>44256</v>
+        <v>44197</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>44257</v>
+        <v>44198</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>44258</v>
+        <v>44199</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>44259</v>
+        <v>44200</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>44260</v>
+        <v>44201</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>44261</v>
+        <v>44202</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>44262</v>
+        <v>44203</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>44263</v>
+        <v>44204</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>44264</v>
+        <v>44205</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>44265</v>
+        <v>44206</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>44266</v>
+        <v>44207</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>44267</v>
+        <v>44208</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>44268</v>
+        <v>44209</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>44269</v>
+        <v>44210</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>44270</v>
+        <v>44211</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>44271</v>
+        <v>44212</v>
       </c>
       <c r="B17" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>44272</v>
+        <v>44213</v>
       </c>
       <c r="B18" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>44273</v>
+        <v>44214</v>
       </c>
       <c r="B19" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>44274</v>
+        <v>44215</v>
       </c>
       <c r="B20" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>44275</v>
+        <v>44216</v>
       </c>
       <c r="B21" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>44276</v>
+        <v>44217</v>
       </c>
       <c r="B22" s="1">
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>44277</v>
+        <v>44218</v>
       </c>
       <c r="B23" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>44278</v>
+        <v>44219</v>
       </c>
       <c r="B24" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>44279</v>
+        <v>44220</v>
       </c>
       <c r="B25" s="1">
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>44280</v>
+        <v>44221</v>
       </c>
       <c r="B26" s="1">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>44281</v>
+        <v>44222</v>
       </c>
       <c r="B27" s="1">
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>44282</v>
+        <v>44223</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>44283</v>
+        <v>44224</v>
       </c>
       <c r="B29" s="1">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>44284</v>
+        <v>44225</v>
       </c>
       <c r="B30" s="1">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>44285</v>
+        <v>44226</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>44286</v>
+        <v>44227</v>
       </c>
       <c r="B32" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>44256</v>
+        <v>44228</v>
       </c>
       <c r="B33" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>44257</v>
+        <v>44229</v>
       </c>
       <c r="B34" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>44258</v>
+        <v>44230</v>
       </c>
       <c r="B35" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>44259</v>
+        <v>44231</v>
       </c>
       <c r="B36" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>44260</v>
+        <v>44232</v>
       </c>
       <c r="B37" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>44261</v>
+        <v>44233</v>
       </c>
       <c r="B38" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>44262</v>
+        <v>44234</v>
       </c>
       <c r="B39" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>44263</v>
+        <v>44235</v>
       </c>
       <c r="B40" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>44264</v>
+        <v>44236</v>
       </c>
       <c r="B41" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>44265</v>
-      </c>
-      <c r="B42" s="4">
-        <v>20</v>
+        <v>44237</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>44266</v>
-      </c>
-      <c r="B43" s="4">
+        <v>44238</v>
+      </c>
+      <c r="B43" s="1">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>44267</v>
-      </c>
-      <c r="B44" s="4">
-        <v>20</v>
+        <v>44239</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44268</v>
-      </c>
-      <c r="B45" s="4">
-        <v>20</v>
+        <v>44240</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>44269</v>
-      </c>
-      <c r="B46" s="4">
+        <v>44241</v>
+      </c>
+      <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>44270</v>
+        <v>44242</v>
       </c>
       <c r="B47" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>44271</v>
+        <v>44243</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>44272</v>
+        <v>44244</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>44273</v>
+        <v>44245</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>44274</v>
+        <v>44246</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>44275</v>
+        <v>44247</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>44276</v>
+        <v>44248</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>44277</v>
+        <v>44249</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>44278</v>
+        <v>44250</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>44279</v>
+        <v>44251</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>44280</v>
+        <v>44252</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>44281</v>
+        <v>44253</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>44282</v>
+        <v>44254</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>44283</v>
+        <v>44255</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>44284</v>
+        <v>44348</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>44285</v>
+        <v>44349</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>44286</v>
+        <v>44350</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>44351</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <v>44352</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <v>44353</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>44354</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>44355</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <v>44356</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>44357</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
+        <v>44358</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <v>44359</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
+        <v>44360</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
+        <v>44361</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
+        <v>44362</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <v>44363</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A77" s="3">
+        <v>44364</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>44365</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <v>44366</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>44367</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>44368</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>44369</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>44370</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>44371</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>44372</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>44373</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>4</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <v>44374</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <v>44375</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>44376</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <v>44377</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <v>44197</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0</v>
+      </c>
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <v>44198</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>44199</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <v>44200</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <v>44201</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <v>44203</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>44204</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>44205</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
+        <v>44206</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>44207</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>44208</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A103" s="3">
+        <v>44209</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A104" s="3">
+        <v>44210</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A105" s="3">
+        <v>44211</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A106" s="3">
+        <v>44212</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A107" s="3">
+        <v>44213</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>44214</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A109" s="3">
+        <v>44215</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>44216</v>
+      </c>
+      <c r="B110" s="1">
+        <v>0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>44217</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A112" s="3">
+        <v>44218</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A113" s="3">
+        <v>44219</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A114" s="3">
+        <v>44220</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A115" s="3">
+        <v>44221</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A116" s="3">
+        <v>44222</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0</v>
+      </c>
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A117" s="3">
+        <v>44223</v>
+      </c>
+      <c r="B117" s="1">
+        <v>0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A118" s="3">
+        <v>44224</v>
+      </c>
+      <c r="B118" s="1">
+        <v>0</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A119" s="3">
+        <v>44225</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0</v>
+      </c>
+      <c r="C119" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A120" s="3">
+        <v>44226</v>
+      </c>
+      <c r="B120" s="1">
+        <v>0</v>
+      </c>
+      <c r="C120" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A121" s="3">
+        <v>44227</v>
+      </c>
+      <c r="B121" s="1">
+        <v>0</v>
+      </c>
+      <c r="C121" t="s">
+        <v>7</v>
+      </c>
+      <c r="D121" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A122" s="3">
+        <v>44228</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A123" s="3">
+        <v>44229</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0</v>
+      </c>
+      <c r="C123" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A124" s="3">
+        <v>44230</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A125" s="3">
+        <v>44231</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A126" s="3">
+        <v>44232</v>
+      </c>
+      <c r="B126" s="1">
+        <v>0</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A127" s="3">
+        <v>44233</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A128" s="3">
+        <v>44234</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A129" s="3">
+        <v>44235</v>
+      </c>
+      <c r="B129" s="1">
+        <v>0</v>
+      </c>
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" t="s">
+        <v>6</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A130" s="3">
+        <v>44236</v>
+      </c>
+      <c r="B130" s="1">
+        <v>0</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" t="s">
+        <v>6</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A131" s="3">
+        <v>44237</v>
+      </c>
+      <c r="B131" s="1">
+        <v>0</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" t="s">
+        <v>6</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A132" s="3">
+        <v>44238</v>
+      </c>
+      <c r="B132" s="1">
+        <v>0</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" t="s">
+        <v>6</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A133" s="3">
+        <v>44239</v>
+      </c>
+      <c r="B133" s="1">
+        <v>0</v>
+      </c>
+      <c r="C133" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133" t="s">
+        <v>6</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A134" s="3">
+        <v>44240</v>
+      </c>
+      <c r="B134" s="1">
+        <v>0</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134" t="s">
+        <v>6</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A135" s="3">
+        <v>44241</v>
+      </c>
+      <c r="B135" s="1">
+        <v>0</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A136" s="3">
+        <v>44242</v>
+      </c>
+      <c r="B136" s="1">
+        <v>0</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" t="s">
+        <v>6</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A137" s="3">
+        <v>44243</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0</v>
+      </c>
+      <c r="C137" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" t="s">
+        <v>6</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A138" s="3">
+        <v>44244</v>
+      </c>
+      <c r="B138" s="1">
+        <v>0</v>
+      </c>
+      <c r="C138" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A139" s="3">
+        <v>44245</v>
+      </c>
+      <c r="B139" s="1">
+        <v>0</v>
+      </c>
+      <c r="C139" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" t="s">
+        <v>6</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A140" s="3">
+        <v>44246</v>
+      </c>
+      <c r="B140" s="1">
+        <v>0</v>
+      </c>
+      <c r="C140" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A141" s="3">
+        <v>44247</v>
+      </c>
+      <c r="B141" s="1">
+        <v>0</v>
+      </c>
+      <c r="C141" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" t="s">
+        <v>6</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A142" s="3">
+        <v>44248</v>
+      </c>
+      <c r="B142" s="1">
+        <v>0</v>
+      </c>
+      <c r="C142" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" t="s">
+        <v>6</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A143" s="3">
+        <v>44249</v>
+      </c>
+      <c r="B143" s="1">
+        <v>0</v>
+      </c>
+      <c r="C143" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A144" s="3">
+        <v>44250</v>
+      </c>
+      <c r="B144" s="1">
+        <v>0</v>
+      </c>
+      <c r="C144" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A145" s="3">
+        <v>44251</v>
+      </c>
+      <c r="B145" s="1">
+        <v>0</v>
+      </c>
+      <c r="C145" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A146" s="3">
+        <v>44252</v>
+      </c>
+      <c r="B146" s="1">
+        <v>0</v>
+      </c>
+      <c r="C146" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A147" s="3">
+        <v>44253</v>
+      </c>
+      <c r="B147" s="1">
+        <v>0</v>
+      </c>
+      <c r="C147" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A148" s="3">
+        <v>44254</v>
+      </c>
+      <c r="B148" s="1">
+        <v>0</v>
+      </c>
+      <c r="C148" t="s">
+        <v>7</v>
+      </c>
+      <c r="D148" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A149" s="3">
+        <v>44255</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0</v>
+      </c>
+      <c r="C149" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" t="s">
+        <v>6</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A150" s="3">
+        <v>44348</v>
+      </c>
+      <c r="B150" s="1">
+        <v>0</v>
+      </c>
+      <c r="C150" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" t="s">
+        <v>6</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A151" s="3">
+        <v>44349</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0</v>
+      </c>
+      <c r="C151" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A152" s="3">
+        <v>44350</v>
+      </c>
+      <c r="B152" s="1">
+        <v>0</v>
+      </c>
+      <c r="C152" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" t="s">
+        <v>6</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A153" s="3">
+        <v>44351</v>
+      </c>
+      <c r="B153" s="1">
+        <v>0</v>
+      </c>
+      <c r="C153" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" t="s">
+        <v>6</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A154" s="3">
+        <v>44352</v>
+      </c>
+      <c r="B154" s="1">
+        <v>0</v>
+      </c>
+      <c r="C154" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" t="s">
+        <v>6</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A155" s="3">
+        <v>44353</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0</v>
+      </c>
+      <c r="C155" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" t="s">
+        <v>6</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A156" s="3">
+        <v>44354</v>
+      </c>
+      <c r="B156" s="1">
+        <v>0</v>
+      </c>
+      <c r="C156" t="s">
+        <v>7</v>
+      </c>
+      <c r="D156" t="s">
+        <v>6</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A157" s="3">
+        <v>44355</v>
+      </c>
+      <c r="B157" s="1">
+        <v>0</v>
+      </c>
+      <c r="C157" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" t="s">
+        <v>6</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A158" s="3">
+        <v>44356</v>
+      </c>
+      <c r="B158" s="1">
+        <v>0</v>
+      </c>
+      <c r="C158" t="s">
+        <v>7</v>
+      </c>
+      <c r="D158" t="s">
+        <v>6</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A159" s="3">
+        <v>44357</v>
+      </c>
+      <c r="B159" s="1">
+        <v>0</v>
+      </c>
+      <c r="C159" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" t="s">
+        <v>6</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A160" s="3">
+        <v>44358</v>
+      </c>
+      <c r="B160" s="1">
+        <v>0</v>
+      </c>
+      <c r="C160" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" t="s">
+        <v>6</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A161" s="3">
+        <v>44359</v>
+      </c>
+      <c r="B161" s="1">
+        <v>0</v>
+      </c>
+      <c r="C161" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A162" s="3">
+        <v>44360</v>
+      </c>
+      <c r="B162" s="1">
+        <v>0</v>
+      </c>
+      <c r="C162" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162" t="s">
+        <v>6</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A163" s="3">
+        <v>44361</v>
+      </c>
+      <c r="B163" s="1">
+        <v>0</v>
+      </c>
+      <c r="C163" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163" t="s">
+        <v>6</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A164" s="3">
+        <v>44362</v>
+      </c>
+      <c r="B164" s="1">
+        <v>0</v>
+      </c>
+      <c r="C164" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A165" s="3">
+        <v>44363</v>
+      </c>
+      <c r="B165" s="1">
+        <v>0</v>
+      </c>
+      <c r="C165" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" t="s">
+        <v>6</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A166" s="3">
+        <v>44364</v>
+      </c>
+      <c r="B166" s="1">
+        <v>0</v>
+      </c>
+      <c r="C166" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A167" s="3">
+        <v>44365</v>
+      </c>
+      <c r="B167" s="1">
+        <v>0</v>
+      </c>
+      <c r="C167" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" t="s">
+        <v>6</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A168" s="3">
+        <v>44366</v>
+      </c>
+      <c r="B168" s="1">
+        <v>0</v>
+      </c>
+      <c r="C168" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A169" s="3">
+        <v>44367</v>
+      </c>
+      <c r="B169" s="1">
+        <v>0</v>
+      </c>
+      <c r="C169" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" t="s">
+        <v>6</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A170" s="3">
+        <v>44368</v>
+      </c>
+      <c r="B170" s="1">
+        <v>0</v>
+      </c>
+      <c r="C170" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" t="s">
+        <v>6</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A171" s="3">
+        <v>44369</v>
+      </c>
+      <c r="B171" s="1">
+        <v>0</v>
+      </c>
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" t="s">
+        <v>6</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A172" s="3">
+        <v>44370</v>
+      </c>
+      <c r="B172" s="1">
+        <v>0</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A173" s="3">
+        <v>44371</v>
+      </c>
+      <c r="B173" s="1">
+        <v>0</v>
+      </c>
+      <c r="C173" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" t="s">
+        <v>6</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A174" s="3">
+        <v>44372</v>
+      </c>
+      <c r="B174" s="1">
+        <v>0</v>
+      </c>
+      <c r="C174" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" t="s">
+        <v>6</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A175" s="3">
+        <v>44373</v>
+      </c>
+      <c r="B175" s="1">
+        <v>0</v>
+      </c>
+      <c r="C175" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" t="s">
+        <v>6</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A176" s="3">
+        <v>44374</v>
+      </c>
+      <c r="B176" s="1">
+        <v>0</v>
+      </c>
+      <c r="C176" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" t="s">
+        <v>6</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A177" s="3">
+        <v>44375</v>
+      </c>
+      <c r="B177" s="1">
+        <v>0</v>
+      </c>
+      <c r="C177" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" t="s">
+        <v>6</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A178" s="3">
+        <v>44376</v>
+      </c>
+      <c r="B178" s="1">
+        <v>0</v>
+      </c>
+      <c r="C178" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" t="s">
+        <v>6</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A179" s="3">
+        <v>44377</v>
+      </c>
+      <c r="B179" s="1">
+        <v>0</v>
+      </c>
+      <c r="C179" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" t="s">
+        <v>6</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A180" s="3"/>
+      <c r="B180" s="1"/>
+      <c r="E180" s="2"/>
+    </row>
+    <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A181" s="3"/>
+      <c r="B181" s="1"/>
+      <c r="E181" s="2"/>
+    </row>
+    <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A182" s="3"/>
+      <c r="B182" s="1"/>
+      <c r="E182" s="2"/>
+    </row>
+    <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A183" s="3"/>
+      <c r="B183" s="1"/>
+      <c r="E183" s="2"/>
+    </row>
+    <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A184" s="3"/>
+      <c r="B184" s="1"/>
+      <c r="E184" s="2"/>
+    </row>
+    <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A185" s="3"/>
+      <c r="B185" s="1"/>
+      <c r="E185" s="2"/>
+    </row>
+    <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A186" s="3"/>
+      <c r="B186" s="1"/>
+      <c r="E186" s="2"/>
+    </row>
+    <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A187" s="3"/>
+      <c r="B187" s="1"/>
+      <c r="E187" s="2"/>
+    </row>
+    <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A188" s="3"/>
+      <c r="B188" s="1"/>
+      <c r="E188" s="2"/>
+    </row>
+    <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A189" s="3"/>
+      <c r="B189" s="1"/>
+      <c r="E189" s="2"/>
+    </row>
+    <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A190" s="3"/>
+      <c r="B190" s="1"/>
+      <c r="E190" s="2"/>
+    </row>
+    <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A191" s="3"/>
+      <c r="B191" s="1"/>
+      <c r="E191" s="2"/>
+    </row>
+    <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A192" s="3"/>
+      <c r="B192" s="1"/>
+      <c r="E192" s="2"/>
+    </row>
+    <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A193" s="3"/>
+      <c r="B193" s="1"/>
+      <c r="E193" s="2"/>
+    </row>
+    <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A194" s="3"/>
+      <c r="B194" s="1"/>
+      <c r="E194" s="2"/>
+    </row>
+    <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A195" s="3"/>
+      <c r="B195" s="1"/>
+      <c r="E195" s="2"/>
+    </row>
+    <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A196" s="3"/>
+      <c r="B196" s="1"/>
+      <c r="E196" s="2"/>
+    </row>
+    <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A197" s="3"/>
+      <c r="B197" s="1"/>
+      <c r="E197" s="2"/>
+    </row>
+    <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A198" s="3"/>
+      <c r="B198" s="1"/>
+      <c r="E198" s="2"/>
+    </row>
+    <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A199" s="3"/>
+      <c r="B199" s="1"/>
+      <c r="E199" s="2"/>
+    </row>
+    <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A200" s="3"/>
+      <c r="B200" s="1"/>
+      <c r="E200" s="2"/>
+    </row>
+    <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A201" s="3"/>
+      <c r="B201" s="1"/>
+      <c r="E201" s="2"/>
+    </row>
+    <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A202" s="3"/>
+      <c r="B202" s="1"/>
+      <c r="E202" s="2"/>
+    </row>
+    <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A203" s="3"/>
+      <c r="B203" s="1"/>
+      <c r="E203" s="2"/>
+    </row>
+    <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A204" s="3"/>
+      <c r="B204" s="1"/>
+      <c r="E204" s="2"/>
+    </row>
+    <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A205" s="3"/>
+      <c r="B205" s="1"/>
+      <c r="E205" s="2"/>
+    </row>
+    <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A206" s="3"/>
+      <c r="B206" s="1"/>
+      <c r="E206" s="2"/>
+    </row>
+    <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A207" s="3"/>
+      <c r="B207" s="1"/>
+      <c r="E207" s="2"/>
+    </row>
+    <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A208" s="3"/>
+      <c r="B208" s="1"/>
+      <c r="E208" s="2"/>
+    </row>
+    <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A209" s="3"/>
+      <c r="B209" s="1"/>
+      <c r="E209" s="2"/>
+    </row>
+    <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A210" s="3"/>
+      <c r="B210" s="1"/>
+      <c r="E210" s="2"/>
+    </row>
+    <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A211" s="3"/>
+      <c r="B211" s="1"/>
+      <c r="E211" s="2"/>
+    </row>
+    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A212" s="3"/>
+      <c r="B212" s="1"/>
+      <c r="E212" s="2"/>
+    </row>
+    <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A213" s="3"/>
+      <c r="B213" s="1"/>
+      <c r="E213" s="2"/>
+    </row>
+    <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A214" s="3"/>
+      <c r="B214" s="1"/>
+      <c r="E214" s="2"/>
+    </row>
+    <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A215" s="3"/>
+      <c r="B215" s="1"/>
+      <c r="E215" s="2"/>
+    </row>
+    <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A216" s="3"/>
+      <c r="B216" s="1"/>
+      <c r="E216" s="2"/>
+    </row>
+    <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A217" s="3"/>
+      <c r="B217" s="1"/>
+      <c r="E217" s="2"/>
+    </row>
+    <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A218" s="3"/>
+      <c r="B218" s="1"/>
+      <c r="E218" s="2"/>
+    </row>
+    <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A219" s="3"/>
+      <c r="B219" s="1"/>
+      <c r="E219" s="2"/>
+    </row>
+    <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A220" s="3"/>
+      <c r="B220" s="1"/>
+      <c r="E220" s="2"/>
+    </row>
+    <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A221" s="3"/>
+      <c r="B221" s="1"/>
+      <c r="E221" s="2"/>
+    </row>
+    <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A222" s="3"/>
+      <c r="B222" s="1"/>
+      <c r="E222" s="2"/>
+    </row>
+    <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A223" s="3"/>
+      <c r="B223" s="1"/>
+      <c r="E223" s="2"/>
+    </row>
+    <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A224" s="3"/>
+      <c r="B224" s="1"/>
+      <c r="E224" s="2"/>
+    </row>
+    <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A225" s="3"/>
+      <c r="B225" s="1"/>
+      <c r="E225" s="2"/>
+    </row>
+    <row r="226" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A226" s="3"/>
+      <c r="B226" s="1"/>
+      <c r="E226" s="2"/>
+    </row>
+    <row r="227" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A227" s="3"/>
+      <c r="B227" s="1"/>
+      <c r="E227" s="2"/>
+    </row>
+    <row r="228" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A228" s="3"/>
+      <c r="B228" s="1"/>
+      <c r="E228" s="2"/>
+    </row>
+    <row r="229" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A229" s="3"/>
+      <c r="B229" s="1"/>
+      <c r="E229" s="2"/>
+    </row>
+    <row r="230" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A230" s="3"/>
+      <c r="B230" s="1"/>
+      <c r="E230" s="2"/>
+    </row>
+    <row r="231" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A231" s="3"/>
+      <c r="B231" s="1"/>
+      <c r="E231" s="2"/>
+    </row>
+    <row r="232" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A232" s="3"/>
+      <c r="B232" s="1"/>
+      <c r="E232" s="2"/>
+    </row>
+    <row r="233" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A233" s="3"/>
+      <c r="B233" s="1"/>
+      <c r="E233" s="2"/>
+    </row>
+    <row r="234" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A234" s="3"/>
+      <c r="B234" s="1"/>
+      <c r="E234" s="2"/>
+    </row>
+    <row r="235" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A235" s="3"/>
+      <c r="B235" s="1"/>
+      <c r="E235" s="2"/>
+    </row>
+    <row r="236" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A236" s="3"/>
+      <c r="B236" s="1"/>
+      <c r="E236" s="2"/>
+    </row>
+    <row r="237" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A237" s="3"/>
+      <c r="B237" s="1"/>
+      <c r="E237" s="2"/>
+    </row>
+    <row r="238" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A238" s="3"/>
+      <c r="B238" s="1"/>
+      <c r="E238" s="2"/>
+    </row>
+    <row r="239" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A239" s="3"/>
+      <c r="B239" s="1"/>
+      <c r="E239" s="2"/>
+    </row>
+    <row r="240" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A240" s="3"/>
+      <c r="B240" s="1"/>
+      <c r="E240" s="2"/>
+    </row>
+    <row r="241" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A241" s="3"/>
+      <c r="B241" s="1"/>
+      <c r="E241" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>